<commit_message>
Changed the format of the xlsx form for Daily Inventory
</commit_message>
<xml_diff>
--- a/SMS/exlTMP/rptDailyInventory.xlsx
+++ b/SMS/exlTMP/rptDailyInventory.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOURCE CODE\SMS\SMS\exlTMP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA1828-6E8B-4A6D-91B9-F2828CB09AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="7500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DailyInventory" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Description</t>
   </si>
@@ -54,13 +60,16 @@
   </si>
   <si>
     <t>ITEMCODE</t>
+  </si>
+  <si>
+    <t>BRANCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,31 +167,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -214,7 +217,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -226,13 +229,21 @@
       <color rgb="FF0099FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,7 +281,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -304,6 +315,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -338,9 +350,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -513,49 +526,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
     <col min="8" max="9" width="8.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="24.75" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="12"/>
+    <row r="2" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -564,49 +579,53 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.16" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>